<commit_message>
Add indication of type of value
</commit_message>
<xml_diff>
--- a/source/cs-core/2014.xlsx
+++ b/source/cs-core/2014.xlsx
@@ -5,67 +5,67 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="427" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="302" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="iso" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="scores" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="parameters" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="indicators" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="score" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="param" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="ind" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName function="false" hidden="false" name="criteria_GreenMFIConts" vbProcedure="false">#ref!</definedName>
-    <definedName function="false" hidden="false" name="dbl_BenchmarkMax" vbProcedure="false">#NAME?</definedName>
-    <definedName function="false" hidden="false" name="dbl_DBWeightP1" vbProcedure="false">#NAME?</definedName>
-    <definedName function="false" hidden="false" name="dbl_DBWeightP2" vbProcedure="false">#NAME?</definedName>
-    <definedName function="false" hidden="false" name="dbl_DBWeightP3" vbProcedure="false">#NAME?</definedName>
-    <definedName function="false" hidden="false" name="dbl_DBWeightP4" vbProcedure="false">#NAME?</definedName>
-    <definedName function="false" hidden="false" name="dbl_ScoreMax" vbProcedure="false">#NAME?</definedName>
-    <definedName function="false" hidden="false" name="DynamicRange_CapBio" vbProcedure="false">OFFSET(#NAME?, 0, 1, 1, #NAME?)</definedName>
-    <definedName function="false" hidden="false" name="DynamicRange_CapGeo" vbProcedure="false">OFFSET(#NAME?, 1, 1, 1, #NAME?)</definedName>
-    <definedName function="false" hidden="false" name="DynamicRange_CapOther" vbProcedure="false">OFFSET(#NAME?, 2, 1, 1, #NAME?)</definedName>
-    <definedName function="false" hidden="false" name="DynamicRange_CapSmHy" vbProcedure="false">OFFSET(#NAME?, 3, 1, 1, #NAME?)</definedName>
-    <definedName function="false" hidden="false" name="DynamicRange_CapSolar" vbProcedure="false">OFFSET(#NAME?, 4, 1, 1, #NAME?)</definedName>
-    <definedName function="false" hidden="false" name="DynamicRange_CapWind" vbProcedure="false">OFFSET(#NAME?, 5, 1, 1, #NAME?)</definedName>
-    <definedName function="false" hidden="false" name="DynamicRange_GenBio" vbProcedure="false">OFFSET(#NAME?, 0, 1, 1, #NAME?)</definedName>
-    <definedName function="false" hidden="false" name="DynamicRange_GenGeo" vbProcedure="false">OFFSET(#NAME?, 1, 1, 1, #NAME?)</definedName>
-    <definedName function="false" hidden="false" name="DynamicRange_GenOther" vbProcedure="false">OFFSET(#NAME?, 2, 1, 1, #NAME?)</definedName>
-    <definedName function="false" hidden="false" name="DynamicRange_GenSmHy" vbProcedure="false">OFFSET(#NAME?, 3, 1, 1, #NAME?)</definedName>
-    <definedName function="false" hidden="false" name="DynamicRange_GenSolar" vbProcedure="false">OFFSET(#NAME?, 4, 1, 1, #NAME?)</definedName>
-    <definedName function="false" hidden="false" name="DynamicRange_GenWind" vbProcedure="false">OFFSET(#NAME?, 5, 1, 1, #NAME?)</definedName>
-    <definedName function="false" hidden="false" name="DynamicRange_InvBiofuels" vbProcedure="false">OFFSET(#NAME?, 0, 1, 1, #NAME?)</definedName>
-    <definedName function="false" hidden="false" name="DynamicRange_InvBiomass" vbProcedure="false">OFFSET(#NAME?, 1, 1, 1, #NAME?)</definedName>
-    <definedName function="false" hidden="false" name="DynamicRange_InvGeo" vbProcedure="false">OFFSET(#NAME?, 2, 1, 1, #NAME?)</definedName>
-    <definedName function="false" hidden="false" name="DynamicRange_InvOtherCE" vbProcedure="false">OFFSET(#NAME?, 6, 1, 1, #NAME?)</definedName>
-    <definedName function="false" hidden="false" name="DynamicRange_InvSmallDist" vbProcedure="false">OFFSET(#NAME?, 7, 1, 1, #NAME?)</definedName>
-    <definedName function="false" hidden="false" name="DynamicRange_InvSmHy" vbProcedure="false">OFFSET(#NAME?, 3, 1, 1, #NAME?)</definedName>
-    <definedName function="false" hidden="false" name="DynamicRange_InvSolar" vbProcedure="false">OFFSET(#NAME?, 4, 1, 1, #NAME?)</definedName>
-    <definedName function="false" hidden="false" name="DynamicRange_InvWind" vbProcedure="false">OFFSET(#NAME?, 5, 1, 1, #NAME?)</definedName>
-    <definedName function="false" hidden="false" name="DynamicRange_Scores" vbProcedure="false">OFFSET(#NAME?, 0, 0, 27, COUNTIF(#NAME?, "&lt;&gt;0"))</definedName>
-    <definedName function="false" hidden="false" name="int_Year" vbProcedure="false">#NAME?</definedName>
-    <definedName function="false" hidden="false" name="list_Countries" vbProcedure="false">#NAME?</definedName>
-    <definedName function="false" hidden="false" name="list_RegionOnGrid" vbProcedure="false">#NAME?</definedName>
+    <definedName function="false" hidden="false" name="dbl_BenchmarkMax" vbProcedure="false">#name?</definedName>
+    <definedName function="false" hidden="false" name="dbl_DBWeightP1" vbProcedure="false">#name?</definedName>
+    <definedName function="false" hidden="false" name="dbl_DBWeightP2" vbProcedure="false">#name?</definedName>
+    <definedName function="false" hidden="false" name="dbl_DBWeightP3" vbProcedure="false">#name?</definedName>
+    <definedName function="false" hidden="false" name="dbl_DBWeightP4" vbProcedure="false">#name?</definedName>
+    <definedName function="false" hidden="false" name="dbl_ScoreMax" vbProcedure="false">#name?</definedName>
+    <definedName function="false" hidden="false" name="DynamicRange_CapBio" vbProcedure="false">OFFSET(#name?, 0, 1, 1, #name?)</definedName>
+    <definedName function="false" hidden="false" name="DynamicRange_CapGeo" vbProcedure="false">OFFSET(#name?, 1, 1, 1, #name?)</definedName>
+    <definedName function="false" hidden="false" name="DynamicRange_CapOther" vbProcedure="false">OFFSET(#name?, 2, 1, 1, #name?)</definedName>
+    <definedName function="false" hidden="false" name="DynamicRange_CapSmHy" vbProcedure="false">OFFSET(#name?, 3, 1, 1, #name?)</definedName>
+    <definedName function="false" hidden="false" name="DynamicRange_CapSolar" vbProcedure="false">OFFSET(#name?, 4, 1, 1, #name?)</definedName>
+    <definedName function="false" hidden="false" name="DynamicRange_CapWind" vbProcedure="false">OFFSET(#name?, 5, 1, 1, #name?)</definedName>
+    <definedName function="false" hidden="false" name="DynamicRange_GenBio" vbProcedure="false">OFFSET(#name?, 0, 1, 1, #name?)</definedName>
+    <definedName function="false" hidden="false" name="DynamicRange_GenGeo" vbProcedure="false">OFFSET(#name?, 1, 1, 1, #name?)</definedName>
+    <definedName function="false" hidden="false" name="DynamicRange_GenOther" vbProcedure="false">OFFSET(#name?, 2, 1, 1, #name?)</definedName>
+    <definedName function="false" hidden="false" name="DynamicRange_GenSmHy" vbProcedure="false">OFFSET(#name?, 3, 1, 1, #name?)</definedName>
+    <definedName function="false" hidden="false" name="DynamicRange_GenSolar" vbProcedure="false">OFFSET(#name?, 4, 1, 1, #name?)</definedName>
+    <definedName function="false" hidden="false" name="DynamicRange_GenWind" vbProcedure="false">OFFSET(#name?, 5, 1, 1, #name?)</definedName>
+    <definedName function="false" hidden="false" name="DynamicRange_InvBiofuels" vbProcedure="false">OFFSET(#name?, 0, 1, 1, #name?)</definedName>
+    <definedName function="false" hidden="false" name="DynamicRange_InvBiomass" vbProcedure="false">OFFSET(#name?, 1, 1, 1, #name?)</definedName>
+    <definedName function="false" hidden="false" name="DynamicRange_InvGeo" vbProcedure="false">OFFSET(#name?, 2, 1, 1, #name?)</definedName>
+    <definedName function="false" hidden="false" name="DynamicRange_InvOtherCE" vbProcedure="false">OFFSET(#name?, 6, 1, 1, #name?)</definedName>
+    <definedName function="false" hidden="false" name="DynamicRange_InvSmallDist" vbProcedure="false">OFFSET(#name?, 7, 1, 1, #name?)</definedName>
+    <definedName function="false" hidden="false" name="DynamicRange_InvSmHy" vbProcedure="false">OFFSET(#name?, 3, 1, 1, #name?)</definedName>
+    <definedName function="false" hidden="false" name="DynamicRange_InvSolar" vbProcedure="false">OFFSET(#name?, 4, 1, 1, #name?)</definedName>
+    <definedName function="false" hidden="false" name="DynamicRange_InvWind" vbProcedure="false">OFFSET(#name?, 5, 1, 1, #name?)</definedName>
+    <definedName function="false" hidden="false" name="DynamicRange_Scores" vbProcedure="false">OFFSET(#name?, 0, 0, 27, COUNTIF(#name?, "&lt;&gt;0"))</definedName>
+    <definedName function="false" hidden="false" name="int_Year" vbProcedure="false">#name?</definedName>
+    <definedName function="false" hidden="false" name="list_Countries" vbProcedure="false">#name?</definedName>
+    <definedName function="false" hidden="false" name="list_RegionOnGrid" vbProcedure="false">#name?</definedName>
     <definedName function="false" hidden="false" name="str_CompareScores" vbProcedure="false">[1]dashboard!#ref!</definedName>
-    <definedName function="false" hidden="false" name="str_Country" vbProcedure="false">#NAME?</definedName>
-    <definedName function="false" hidden="false" name="str_GridStatus" vbProcedure="false">#NAME?</definedName>
-    <definedName function="false" hidden="false" name="str_Hyperlink101" vbProcedure="false">#NAME?</definedName>
-    <definedName function="false" hidden="false" name="str_Hyperlink102" vbProcedure="false">#NAME?</definedName>
-    <definedName function="false" hidden="false" name="str_Hyperlink103" vbProcedure="false">#NAME?</definedName>
-    <definedName function="false" hidden="false" name="str_Hyperlink105" vbProcedure="false">#NAME?</definedName>
-    <definedName function="false" hidden="false" name="str_Hyperlink107" vbProcedure="false">#NAME?</definedName>
-    <definedName function="false" hidden="false" name="str_Hyperlink109" vbProcedure="false">#NAME?</definedName>
-    <definedName function="false" hidden="false" name="str_Hyperlink201" vbProcedure="false">#NAME?</definedName>
-    <definedName function="false" hidden="false" name="str_Hyperlink209" vbProcedure="false">#NAME?</definedName>
-    <definedName function="false" hidden="false" name="str_Hyperlink301" vbProcedure="false">#NAME?</definedName>
-    <definedName function="false" hidden="false" name="str_Hyperlink302" vbProcedure="false">#NAME?</definedName>
-    <definedName function="false" hidden="false" name="str_Hyperlink303" vbProcedure="false">#NAME?</definedName>
-    <definedName function="false" hidden="false" name="str_Hyperlink304" vbProcedure="false">#NAME?</definedName>
-    <definedName function="false" hidden="false" name="str_Hyperlink305" vbProcedure="false">#NAME?</definedName>
-    <definedName function="false" hidden="false" name="str_OptionInvType" vbProcedure="false">#NAME?</definedName>
-    <definedName function="false" hidden="false" name="str_WeightScenario" vbProcedure="false">#NAME?</definedName>
+    <definedName function="false" hidden="false" name="str_Country" vbProcedure="false">#name?</definedName>
+    <definedName function="false" hidden="false" name="str_GridStatus" vbProcedure="false">#name?</definedName>
+    <definedName function="false" hidden="false" name="str_Hyperlink101" vbProcedure="false">#name?</definedName>
+    <definedName function="false" hidden="false" name="str_Hyperlink102" vbProcedure="false">#name?</definedName>
+    <definedName function="false" hidden="false" name="str_Hyperlink103" vbProcedure="false">#name?</definedName>
+    <definedName function="false" hidden="false" name="str_Hyperlink105" vbProcedure="false">#name?</definedName>
+    <definedName function="false" hidden="false" name="str_Hyperlink107" vbProcedure="false">#name?</definedName>
+    <definedName function="false" hidden="false" name="str_Hyperlink109" vbProcedure="false">#name?</definedName>
+    <definedName function="false" hidden="false" name="str_Hyperlink201" vbProcedure="false">#name?</definedName>
+    <definedName function="false" hidden="false" name="str_Hyperlink209" vbProcedure="false">#name?</definedName>
+    <definedName function="false" hidden="false" name="str_Hyperlink301" vbProcedure="false">#name?</definedName>
+    <definedName function="false" hidden="false" name="str_Hyperlink302" vbProcedure="false">#name?</definedName>
+    <definedName function="false" hidden="false" name="str_Hyperlink303" vbProcedure="false">#name?</definedName>
+    <definedName function="false" hidden="false" name="str_Hyperlink304" vbProcedure="false">#name?</definedName>
+    <definedName function="false" hidden="false" name="str_Hyperlink305" vbProcedure="false">#name?</definedName>
+    <definedName function="false" hidden="false" name="str_OptionInvType" vbProcedure="false">#name?</definedName>
+    <definedName function="false" hidden="false" name="str_WeightScenario" vbProcedure="false">#name?</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">iso!$A$1:$B$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">parameters!$A$1:$D$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">indicators!$A$1:$D$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">param!$A$1:$D$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">ind!$A$1:$D$1</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
 </workbook>
@@ -494,7 +494,7 @@
     <t>ZA</t>
   </si>
   <si>
-    <t>Sri Lanka </t>
+    <t>Sri Lanka</t>
   </si>
   <si>
     <t>LK</t>
@@ -676,7 +676,7 @@
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Normal 2" xfId="20" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Normal 2" xfId="20" builtinId="54" customBuiltin="true"/>
   </cellStyles>
 </styleSheet>
 </file>
@@ -684,7 +684,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
-    <tabColor rgb="00FFFFFF"/>
+    <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:B81"/>
@@ -1361,7 +1361,7 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
-    <tabColor rgb="00FFFFFF"/>
+    <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:D81"/>
@@ -2527,7 +2527,7 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
-    <tabColor rgb="00FFFFFF"/>
+    <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:D321"/>
@@ -7053,7 +7053,7 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
-    <tabColor rgb="00FFFFFF"/>
+    <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:D4241"/>

</xml_diff>

<commit_message>
Correct the iso code for DR Congo
</commit_message>
<xml_diff>
--- a/source/cs-core/2014.xlsx
+++ b/source/cs-core/2014.xlsx
@@ -257,7 +257,7 @@
     <t>Democratic Republic of Congo</t>
   </si>
   <si>
-    <t>CG</t>
+    <t>CD</t>
   </si>
   <si>
     <t>Dominican Republic</t>
@@ -676,7 +676,7 @@
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Excel Built-in Normal 2" xfId="20" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Normal 2" xfId="20" builtinId="54" customBuiltin="true"/>
   </cellStyles>
 </styleSheet>
 </file>
@@ -689,8 +689,8 @@
   </sheetPr>
   <dimension ref="A1:B81"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B25" activeCellId="0" sqref="B25"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C31" activeCellId="1" sqref="C161:C213 C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1366,8 +1366,8 @@
   </sheetPr>
   <dimension ref="A1:D81"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A45" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C68" activeCellId="1" sqref="C161:C213 C68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -2533,7 +2533,7 @@
   <dimension ref="A1:D321"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
+      <selection pane="topLeft" activeCell="C14" activeCellId="1" sqref="C161:C213 C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -2648,7 +2648,7 @@
         <v>1</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>116</v>
+        <v>60</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>117</v>
@@ -7058,8 +7058,8 @@
   </sheetPr>
   <dimension ref="A1:D4241"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F37" activeCellId="0" sqref="F37"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F22" activeCellId="1" sqref="C161:C213 F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>

</xml_diff>

<commit_message>
Correct small bugs in country codes
</commit_message>
<xml_diff>
--- a/source/cs-core/2014.xlsx
+++ b/source/cs-core/2014.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="302" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="302" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="iso" sheetId="1" state="visible" r:id="rId2"/>
@@ -227,7 +227,7 @@
     <t>China :: Xinjiang</t>
   </si>
   <si>
-    <t>CN-65 </t>
+    <t>CN-65</t>
   </si>
   <si>
     <t>China :: Yunnan</t>
@@ -676,7 +676,7 @@
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Excel Built-in Excel Built-in Normal 2" xfId="20" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Normal 2" xfId="20" builtinId="54" customBuiltin="true"/>
   </cellStyles>
 </styleSheet>
 </file>
@@ -690,7 +690,7 @@
   <dimension ref="A1:B81"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C31" activeCellId="1" sqref="C161:C213 C31"/>
+      <selection pane="topLeft" activeCell="B27" activeCellId="1" sqref="C8 B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1366,8 +1366,8 @@
   </sheetPr>
   <dimension ref="A1:D81"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A45" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C68" activeCellId="1" sqref="C161:C213 C68"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A45" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C68" activeCellId="1" sqref="C8 C68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -2533,7 +2533,7 @@
   <dimension ref="A1:D321"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C14" activeCellId="1" sqref="C161:C213 C14"/>
+      <selection pane="topLeft" activeCell="C14" activeCellId="1" sqref="C8 C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -7058,8 +7058,8 @@
   </sheetPr>
   <dimension ref="A1:D4241"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F22" activeCellId="1" sqref="C161:C213 F22"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C24" activeCellId="1" sqref="C8 C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>

</xml_diff>